<commit_message>
improve target AFR map based on test-riding
</commit_message>
<xml_diff>
--- a/misc/target fuel table.xlsx
+++ b/misc/target fuel table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d1da377b1bb6b6b/motor/rsv mille/tuning/logger/diy-afr-tuning/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{67DE71FE-788B-47BE-9AA1-22C18A8A9B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C881F344-D213-4E8D-8BEF-418AF5426568}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="8_{67DE71FE-788B-47BE-9AA1-22C18A8A9B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D97C9274-5BC8-44F2-900B-D8579D0A4FFA}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{74104BE9-9BDE-4BE9-9A9A-5B5EE6160832}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -500,35 +500,35 @@
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:J17" si="1">MIN(MAX($M$2+($O$2*(C$1/$N$5)^$M$5)+($O$2*($B2/$N$8)^$M$8),$N$2),$M$2)</f>
-        <v>14.496081485242474</v>
+        <v>14.495704246529314</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" si="1"/>
-        <v>14.227380908391586</v>
+        <v>14.09836121654463</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" si="1"/>
-        <v>14.071228569517514</v>
+        <v>13.922457494557523</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" si="1"/>
-        <v>13.895248729810481</v>
+        <v>13.739300622477669</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" si="1"/>
-        <v>13.646375653792553</v>
+        <v>13.497623680855883</v>
       </c>
       <c r="H2" s="1">
         <f t="shared" si="1"/>
-        <v>13.29441597437849</v>
+        <v>13.178729044534537</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" si="1"/>
-        <v>13.024347813683654</v>
+        <v>12.94683733827806</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" si="1"/>
-        <v>12.796669822342633</v>
+        <v>12.757945049205475</v>
       </c>
       <c r="K2" s="1">
         <f>MIN(MAX($M$2+($O$2*(K$1/$N$5)^$M$5)+($O$2*($B2/$N$8)^$M$8),$N$2),$M$2)</f>
@@ -552,35 +552,35 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" si="1"/>
-        <v>14.48726870799217</v>
+        <v>14.48604305579712</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="1"/>
-        <v>14.218568131141282</v>
+        <v>14.088700025812436</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" si="1"/>
-        <v>14.06241579226721</v>
+        <v>13.91279630382533</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="1"/>
-        <v>13.886435952560177</v>
+        <v>13.729639431745476</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" si="1"/>
-        <v>13.637562876542249</v>
+        <v>13.487962490123689</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" si="1"/>
-        <v>13.285603197128186</v>
+        <v>13.169067853802343</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" si="1"/>
-        <v>13.01553503643335</v>
+        <v>12.937176147545866</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" si="1"/>
-        <v>12.787857045092329</v>
+        <v>12.748283858473281</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K22" si="2">MIN(MAX($M$2+($O$2*(K$1/$N$5)^$M$5)+($O$2*($B3/$N$8)^$M$8),$N$2),$M$2)</f>
@@ -594,35 +594,35 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="1"/>
-        <v>14.47463542325368</v>
+        <v>14.472193554105871</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>14.205934846402792</v>
+        <v>14.074850524121187</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="1"/>
-        <v>14.04978250752872</v>
+        <v>13.898946802134081</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
-        <v>13.873802667821687</v>
+        <v>13.715789930054227</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>13.62492959180376</v>
+        <v>13.47411298843244</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>13.272969912389696</v>
+        <v>13.155218352111094</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>13.002901751694861</v>
+        <v>12.923326645854617</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
-        <v>12.775223760353839</v>
+        <v>12.734434356782032</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
@@ -642,42 +642,42 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
-        <v>14.458635910231719</v>
+        <v>14.454653754501601</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>14.189935333380831</v>
+        <v>14.057310724516917</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="1"/>
-        <v>14.033782994506758</v>
+        <v>13.88140700252981</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>13.857803154799726</v>
+        <v>13.698250130449956</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>13.608930078781798</v>
+        <v>13.45657318882817</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>13.256970399367734</v>
+        <v>13.137678552506824</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>12.986902238672899</v>
+        <v>12.905786846250347</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>12.759224247331877</v>
+        <v>12.716894557177762</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
         <v>12.6</v>
       </c>
       <c r="M5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N5">
         <v>100</v>
@@ -690,35 +690,35 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>14.439553592575967</v>
+        <v>14.433734366067247</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>14.170853015725079</v>
+        <v>14.036391336082563</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>14.014700676851007</v>
+        <v>13.860487614095456</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>13.838720837143974</v>
+        <v>13.677330742015602</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>13.589847761126046</v>
+        <v>13.435653800393816</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>13.237888081711983</v>
+        <v>13.116759164072469</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>12.967819921017147</v>
+        <v>12.884867457815993</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>12.740141929676126</v>
+        <v>12.695975168743407</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
@@ -732,35 +732,35 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>14.417590247020961</v>
+        <v>14.409656590753377</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>14.148889670170073</v>
+        <v>14.012313560768693</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>13.992737331296</v>
+        <v>13.836409838781586</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
-        <v>13.816757491588968</v>
+        <v>13.653252966701732</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>13.56788441557104</v>
+        <v>13.411576025079945</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>13.215924736156976</v>
+        <v>13.092681388758599</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>12.945856575462141</v>
+        <v>12.860789682502123</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>12.718178584121119</v>
+        <v>12.671897393429537</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
@@ -780,35 +780,35 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>14.392900324559632</v>
+        <v>14.38258974867998</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>14.124199747708744</v>
+        <v>13.985246718695295</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>13.968047408834671</v>
+        <v>13.809342996708189</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>13.792067569127639</v>
+        <v>13.626186124628335</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>13.543194493109711</v>
+        <v>13.384509183006548</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>13.191234813695647</v>
+        <v>13.065614546685202</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>12.921166653000812</v>
+        <v>12.833722840428726</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>12.69348866165979</v>
+        <v>12.64483055135614</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
@@ -818,7 +818,7 @@
         <v>1.7</v>
       </c>
       <c r="N8">
-        <v>19000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -828,35 +828,35 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>14.365607675850475</v>
+        <v>14.352669613712667</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>14.096907098999587</v>
+        <v>13.955326583727983</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
-        <v>13.940754760125515</v>
+        <v>13.779422861740876</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>13.764774920418482</v>
+        <v>13.596265989661022</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>13.515901844400554</v>
+        <v>13.354589048039236</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
-        <v>13.163942164986491</v>
+        <v>13.035694411717889</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>12.893874004291655</v>
+        <v>12.803802705461413</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>12.666196012950634</v>
+        <v>12.614910416388827</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
@@ -870,35 +870,35 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>14.335814895864726</v>
+        <v>14.320008657726889</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>14.067114319013838</v>
+        <v>13.922665627742205</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>13.910961980139765</v>
+        <v>13.746761905755099</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>13.734982140432733</v>
+        <v>13.563605033675245</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>13.486109064414805</v>
+        <v>13.321928092053458</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>13.134149385000741</v>
+        <v>13.003033455732112</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>12.864081224305906</v>
+        <v>12.771141749475635</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v>12.636403232964884</v>
+        <v>12.6</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="2"/>
@@ -912,35 +912,35 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>14.303609042874816</v>
+        <v>14.284702320168227</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>14.034908466023928</v>
+        <v>13.887359290183543</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>13.878756127149856</v>
+        <v>13.711455568196437</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
-        <v>13.702776287442823</v>
+        <v>13.528298696116583</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>13.453903211424896</v>
+        <v>13.286621754494796</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>13.101943532010832</v>
+        <v>12.96772711817345</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>12.831875371315997</v>
+        <v>12.735835411916973</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>12.604197379974975</v>
+        <v>12.6</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="2"/>
@@ -954,31 +954,31 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>14.269065376023589</v>
+        <v>14.246833105440533</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>14.000364799172701</v>
+        <v>13.849490075455847</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>13.844212460298628</v>
+        <v>13.673586353468743</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>13.668232620591596</v>
+        <v>13.490429481388887</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>13.419359544573668</v>
+        <v>13.2487525397671</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>13.067399865159604</v>
+        <v>12.929857903445754</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
-        <v>12.797331704464769</v>
+        <v>12.697966197189277</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="1"/>
@@ -996,31 +996,31 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>14.232249922638601</v>
+        <v>14.206473397377753</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>13.963549345787714</v>
+        <v>13.809130367393069</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>13.807397006913641</v>
+        <v>13.633226645405962</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>13.631417167206608</v>
+        <v>13.450069773326108</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>13.382544091188681</v>
+        <v>13.208392831704321</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>13.030584411774617</v>
+        <v>12.889498195382975</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>12.760516251079782</v>
+        <v>12.657606489126499</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="1"/>
@@ -1038,31 +1038,31 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>14.193221312100063</v>
+        <v>14.163687469659862</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>13.924520735249175</v>
+        <v>13.766344439675178</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>13.768368396375102</v>
+        <v>13.590440717688072</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>13.59238855666807</v>
+        <v>13.407283845608218</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>13.343515480650142</v>
+        <v>13.165606903986431</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>12.991555801236078</v>
+        <v>12.846712267665085</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="1"/>
-        <v>12.721487640541243</v>
+        <v>12.614820561408608</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="1"/>
@@ -1080,31 +1080,31 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>14.152032127898343</v>
+        <v>14.118532968034103</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>13.883331551047455</v>
+        <v>13.721189938049418</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>13.727179212173382</v>
+        <v>13.545286216062312</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>13.55119937246635</v>
+        <v>13.362129343982458</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>13.302326296448422</v>
+        <v>13.120452402360671</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>12.950366617034359</v>
+        <v>12.801557766039325</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="1"/>
-        <v>12.680298456339523</v>
+        <v>12.6</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="1"/>
@@ -1122,31 +1122,31 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>14.108729930849009</v>
+        <v>14.071062032035774</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>13.840029353998121</v>
+        <v>13.67371900205109</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>13.683877015124049</v>
+        <v>13.497815280063984</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>13.507897175417016</v>
+        <v>13.31465840798413</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>13.259024099399088</v>
+        <v>13.072981466362343</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>12.907064419985025</v>
+        <v>12.754086830040997</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="1"/>
-        <v>12.636996259290189</v>
+        <v>12.6</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="1"/>
@@ -1164,27 +1164,27 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>14.063358050630658</v>
+        <v>14.021322162728099</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>13.79465747377977</v>
+        <v>13.623979132743415</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>13.638505134905698</v>
+        <v>13.448075410756308</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
-        <v>13.462525295198665</v>
+        <v>13.264918538676454</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>13.213652219180737</v>
+        <v>13.023241597054668</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>12.861692539766674</v>
+        <v>12.704346960733321</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="1"/>
@@ -1206,27 +1206,27 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" ref="C18:J22" si="4">MIN(MAX($M$2+($O$2*(C$1/$N$5)^$M$5)+($O$2*($B18/$N$8)^$M$8),$N$2),$M$2)</f>
-        <v>14.015956209668607</v>
+        <v>13.969356906647702</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="4"/>
-        <v>13.747255632817719</v>
+        <v>13.572013876663018</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="4"/>
-        <v>13.591103293943647</v>
+        <v>13.396110154675911</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="4"/>
-        <v>13.415123454236614</v>
+        <v>13.212953282596057</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="4"/>
-        <v>13.166250378218686</v>
+        <v>12.971276340974271</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="4"/>
-        <v>12.814290698804623</v>
+        <v>12.652381704652925</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="4"/>
@@ -1248,27 +1248,27 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="4"/>
-        <v>13.9665610228805</v>
+        <v>13.915206403661164</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="4"/>
-        <v>13.697860446029612</v>
+        <v>13.51786337367648</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="4"/>
-        <v>13.541708107155539</v>
+        <v>13.341959651689374</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="4"/>
-        <v>13.365728267448507</v>
+        <v>13.15880277960952</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="4"/>
-        <v>13.116855191430579</v>
+        <v>12.917125837987733</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="4"/>
-        <v>12.764895512016516</v>
+        <v>12.6</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="4"/>
@@ -1290,27 +1290,27 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="4"/>
-        <v>13.915206403661164</v>
+        <v>13.858907832034369</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="4"/>
-        <v>13.646505826810277</v>
+        <v>13.461564802049685</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="4"/>
-        <v>13.490353487936204</v>
+        <v>13.285661080062578</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="4"/>
-        <v>13.314373648229171</v>
+        <v>13.102504207982724</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="4"/>
-        <v>13.065500572211244</v>
+        <v>12.860827266360937</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="4"/>
-        <v>12.71354089279718</v>
+        <v>12.6</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="4"/>
@@ -1332,27 +1332,27 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="4"/>
-        <v>13.861923897809497</v>
+        <v>13.800495774506819</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="4"/>
-        <v>13.593223320958609</v>
+        <v>13.403152744522135</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="4"/>
-        <v>13.437070982084537</v>
+        <v>13.227249022535029</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="4"/>
-        <v>13.261091142377504</v>
+        <v>13.044092150455175</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="4"/>
-        <v>13.012218066359576</v>
+        <v>12.802415208833388</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="4"/>
-        <v>12.660258386945513</v>
+        <v>12.6</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="4"/>
@@ -1374,27 +1374,27 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" si="4"/>
-        <v>13.806742961221204</v>
+        <v>13.740002522718086</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="4"/>
-        <v>13.538042384370314</v>
+        <v>13.342659492733402</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="4"/>
-        <v>13.381890045496242</v>
+        <v>13.166755770746295</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="4"/>
-        <v>13.205910205789209</v>
+        <v>12.983598898666441</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="4"/>
-        <v>12.957037129771283</v>
+        <v>12.741921957044655</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="4"/>
-        <v>12.605077450357218</v>
+        <v>12.6</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="4"/>

</xml_diff>